<commit_message>
removed cocaine and cannabis features
</commit_message>
<xml_diff>
--- a/Other dataset/Other Dataset/Feature map.xlsx
+++ b/Other dataset/Other Dataset/Feature map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\Year 4 work\Applied-Data-Science-Coursework\Applied-Data-Science-Coursework\Other dataset\Other Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7BDD827-C197-4098-9548-D366712C9B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CDCD9E-47CD-4EF9-9490-B2A6A62E4093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
   <si>
     <t>Variable Code</t>
   </si>
@@ -323,12 +323,6 @@
     <t>How many times have you had five or more alcoholic drinks at a time in the last 12 months?</t>
   </si>
   <si>
-    <t>Have you ever taken any of the following? Cannabis/Marijuana/Weed</t>
-  </si>
-  <si>
-    <t>Have you ever taken any of the following? Cocaine powder</t>
-  </si>
-  <si>
     <t>Have you ever taken any of the following? Acid/LSD</t>
   </si>
   <si>
@@ -485,12 +479,6 @@
     <t>AlchDrinkExcsNum</t>
   </si>
   <si>
-    <t>CannabisY/N</t>
-  </si>
-  <si>
-    <t>CocaineY/N</t>
-  </si>
-  <si>
     <t>AcidY/N</t>
   </si>
   <si>
@@ -522,12 +510,6 @@
   </si>
   <si>
     <t>SocialmedAddict</t>
-  </si>
-  <si>
-    <t>GCDRAN00</t>
-  </si>
-  <si>
-    <t>GCDRBN00</t>
   </si>
 </sst>
 </file>
@@ -845,10 +827,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="G45" sqref="G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,14 +856,14 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C2" t="s">
         <v>55</v>
       </c>
       <c r="J2" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,B2:B55)</f>
-        <v>Age,Sex,LikeMusic,LikeTV,LikeDrawing,LikeComputer,LikeOutSport,LikeInSport,FriendCount,LikeFriendPlay,LikeAlone,FunFamily,LikeSchool,SadSchool,TiredSchool,FedSchool,FriendTalk,Bullied,BullyOthers,ChildLeftOut,EverHomeless,CurrHomeless,MumCont,MumSee,MumSpeak,DadCont,DadSee,DadSpeak,agg_score,AgeDepDiag,DeprsTreatCurr,DeprsTreat,FirstCigAge,FirstAlchAge,FirstAlchDrinkAge,AlchDrinkYr,AlchDrinkMon,AlchDrinkExcs,AlchDrinkExcsAge,AlchDrinkExcsNum,CannabisY/N,CocaineY/N,AcidY/N,EcstasyY/N,SpeedY/N,SemeronY/N,KetamineY/N,MephedroneY/N,PsychoactiveY/N,SpeedY/N,FriendSpend,GamesSpend,SocialmedSpend,SocialmedAddict</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,B2:B53)</f>
+        <v>Age,Sex,LikeMusic,LikeTV,LikeDrawing,LikeComputer,LikeOutSport,LikeInSport,FriendCount,LikeFriendPlay,LikeAlone,FunFamily,LikeSchool,SadSchool,TiredSchool,FedSchool,FriendTalk,Bullied,BullyOthers,ChildLeftOut,EverHomeless,CurrHomeless,MumCont,MumSee,MumSpeak,DadCont,DadSee,DadSpeak,agg_score,AgeDepDiag,DeprsTreatCurr,DeprsTreat,FirstCigAge,FirstAlchAge,FirstAlchDrinkAge,AlchDrinkYr,AlchDrinkMon,AlchDrinkExcs,AlchDrinkExcsAge,AlchDrinkExcsNum,AcidY/N,EcstasyY/N,SpeedY/N,SemeronY/N,KetamineY/N,MephedroneY/N,PsychoactiveY/N,SpeedY/N,FriendSpend,GamesSpend,SocialmedSpend,SocialmedAddict</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -889,7 +871,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
         <v>56</v>
@@ -900,7 +882,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
@@ -911,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>58</v>
@@ -922,7 +904,7 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C6" t="s">
         <v>59</v>
@@ -933,7 +915,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C7" t="s">
         <v>60</v>
@@ -944,7 +926,7 @@
         <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C8" t="s">
         <v>61</v>
@@ -955,7 +937,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>62</v>
@@ -966,7 +948,7 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>63</v>
@@ -977,7 +959,7 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C11" t="s">
         <v>64</v>
@@ -988,7 +970,7 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C12" t="s">
         <v>65</v>
@@ -999,7 +981,7 @@
         <v>14</v>
       </c>
       <c r="B13" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C13" t="s">
         <v>66</v>
@@ -1010,7 +992,7 @@
         <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C14" t="s">
         <v>67</v>
@@ -1021,7 +1003,7 @@
         <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C15" t="s">
         <v>68</v>
@@ -1032,7 +1014,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C16" t="s">
         <v>69</v>
@@ -1043,7 +1025,7 @@
         <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C17" t="s">
         <v>70</v>
@@ -1054,7 +1036,7 @@
         <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C18" t="s">
         <v>71</v>
@@ -1065,7 +1047,7 @@
         <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C19" t="s">
         <v>72</v>
@@ -1076,7 +1058,7 @@
         <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
         <v>73</v>
@@ -1087,7 +1069,7 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
         <v>74</v>
@@ -1098,7 +1080,7 @@
         <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C22" t="s">
         <v>75</v>
@@ -1109,7 +1091,7 @@
         <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C23" t="s">
         <v>76</v>
@@ -1120,7 +1102,7 @@
         <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C24" t="s">
         <v>77</v>
@@ -1131,7 +1113,7 @@
         <v>26</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C25" t="s">
         <v>78</v>
@@ -1142,7 +1124,7 @@
         <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C26" t="s">
         <v>79</v>
@@ -1153,7 +1135,7 @@
         <v>28</v>
       </c>
       <c r="B27" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C27" t="s">
         <v>80</v>
@@ -1164,7 +1146,7 @@
         <v>29</v>
       </c>
       <c r="B28" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C28" t="s">
         <v>81</v>
@@ -1175,7 +1157,7 @@
         <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C29" t="s">
         <v>82</v>
@@ -1186,7 +1168,7 @@
         <v>31</v>
       </c>
       <c r="B30" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C30" t="s">
         <v>83</v>
@@ -1197,7 +1179,7 @@
         <v>32</v>
       </c>
       <c r="B31" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C31" t="s">
         <v>84</v>
@@ -1208,7 +1190,7 @@
         <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C32" t="s">
         <v>85</v>
@@ -1219,7 +1201,7 @@
         <v>34</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C33" t="s">
         <v>86</v>
@@ -1230,7 +1212,7 @@
         <v>35</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C34" t="s">
         <v>87</v>
@@ -1241,7 +1223,7 @@
         <v>36</v>
       </c>
       <c r="B35" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C35" t="s">
         <v>88</v>
@@ -1252,7 +1234,7 @@
         <v>37</v>
       </c>
       <c r="B36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C36" t="s">
         <v>89</v>
@@ -1263,7 +1245,7 @@
         <v>38</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
         <v>90</v>
@@ -1274,7 +1256,7 @@
         <v>39</v>
       </c>
       <c r="B38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C38" t="s">
         <v>91</v>
@@ -1285,7 +1267,7 @@
         <v>40</v>
       </c>
       <c r="B39" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C39" t="s">
         <v>92</v>
@@ -1296,7 +1278,7 @@
         <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C40" t="s">
         <v>93</v>
@@ -1307,7 +1289,7 @@
         <v>42</v>
       </c>
       <c r="B41" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C41" t="s">
         <v>94</v>
@@ -1315,10 +1297,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>162</v>
+        <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C42" t="s">
         <v>95</v>
@@ -1326,10 +1308,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>163</v>
+        <v>44</v>
       </c>
       <c r="B43" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C43" t="s">
         <v>96</v>
@@ -1337,10 +1319,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C44" t="s">
         <v>97</v>
@@ -1348,10 +1330,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C45" t="s">
         <v>98</v>
@@ -1359,10 +1341,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C46" t="s">
         <v>99</v>
@@ -1370,10 +1352,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B47" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C47" t="s">
         <v>100</v>
@@ -1381,10 +1363,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B48" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C48" t="s">
         <v>101</v>
@@ -1392,10 +1374,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B49" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C49" t="s">
         <v>102</v>
@@ -1403,10 +1385,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C50" t="s">
         <v>103</v>
@@ -1414,10 +1396,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B51" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C51" t="s">
         <v>104</v>
@@ -1425,10 +1407,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B52" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" t="s">
         <v>105</v>
@@ -1436,35 +1418,13 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B53" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C53" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>53</v>
-      </c>
-      <c r="B54" t="s">
-        <v>160</v>
-      </c>
-      <c r="C54" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>54</v>
-      </c>
-      <c r="B55" t="s">
-        <v>161</v>
-      </c>
-      <c r="C55" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new features to combined dataset
added features from teacher & parent surveys
</commit_message>
<xml_diff>
--- a/Other dataset/Other Dataset/Feature map.xlsx
+++ b/Other dataset/Other Dataset/Feature map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Downloads\Year 4 work\Applied-Data-Science-Coursework\Applied-Data-Science-Coursework\Other dataset\Other Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12CDCD9E-47CD-4EF9-9490-B2A6A62E4093}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4B8875-79BA-4269-AFBA-DB04C8E088E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,8 +35,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="185">
   <si>
     <t>Variable Code</t>
   </si>
@@ -365,151 +387,232 @@
     <t>Sex</t>
   </si>
   <si>
-    <t>LikeMusic</t>
-  </si>
-  <si>
-    <t>LikeTV</t>
-  </si>
-  <si>
-    <t>LikeDrawing</t>
-  </si>
-  <si>
-    <t>LikeComputer</t>
-  </si>
-  <si>
-    <t>LikeOutSport</t>
-  </si>
-  <si>
-    <t>LikeInSport</t>
-  </si>
-  <si>
-    <t>FriendCount</t>
-  </si>
-  <si>
-    <t>LikeFriendPlay</t>
-  </si>
-  <si>
-    <t>LikeAlone</t>
-  </si>
-  <si>
-    <t>FunFamily</t>
-  </si>
-  <si>
-    <t>LikeSchool</t>
-  </si>
-  <si>
-    <t>SadSchool</t>
-  </si>
-  <si>
-    <t>TiredSchool</t>
-  </si>
-  <si>
-    <t>FedSchool</t>
-  </si>
-  <si>
-    <t>FriendTalk</t>
-  </si>
-  <si>
-    <t>Bullied</t>
-  </si>
-  <si>
-    <t>BullyOthers</t>
-  </si>
-  <si>
-    <t>ChildLeftOut</t>
-  </si>
-  <si>
-    <t>EverHomeless</t>
-  </si>
-  <si>
-    <t>CurrHomeless</t>
-  </si>
-  <si>
-    <t>MumSpeak</t>
-  </si>
-  <si>
-    <t>MumSee</t>
-  </si>
-  <si>
-    <t>MumCont</t>
-  </si>
-  <si>
-    <t>DadCont</t>
-  </si>
-  <si>
-    <t>DadSee</t>
-  </si>
-  <si>
-    <t>DadSpeak</t>
-  </si>
-  <si>
-    <t>agg_score</t>
-  </si>
-  <si>
-    <t>AgeDepDiag</t>
-  </si>
-  <si>
-    <t>DeprsTreatCurr</t>
-  </si>
-  <si>
-    <t>DeprsTreat</t>
-  </si>
-  <si>
-    <t>FirstCigAge</t>
-  </si>
-  <si>
-    <t>FirstAlchAge</t>
-  </si>
-  <si>
-    <t>FirstAlchDrinkAge</t>
-  </si>
-  <si>
-    <t>AlchDrinkYr</t>
-  </si>
-  <si>
-    <t>AlchDrinkMon</t>
-  </si>
-  <si>
-    <t>AlchDrinkExcs</t>
-  </si>
-  <si>
-    <t>AlchDrinkExcsAge</t>
-  </si>
-  <si>
-    <t>AlchDrinkExcsNum</t>
-  </si>
-  <si>
-    <t>AcidY/N</t>
-  </si>
-  <si>
-    <t>EcstasyY/N</t>
-  </si>
-  <si>
-    <t>SpeedY/N</t>
-  </si>
-  <si>
-    <t>SemeronY/N</t>
-  </si>
-  <si>
-    <t>KetamineY/N</t>
-  </si>
-  <si>
-    <t>MephedroneY/N</t>
-  </si>
-  <si>
-    <t>PsychoactiveY/N</t>
-  </si>
-  <si>
-    <t>FriendSpend</t>
-  </si>
-  <si>
-    <t>GamesSpend</t>
-  </si>
-  <si>
-    <t>SocialmedSpend</t>
-  </si>
-  <si>
-    <t>SocialmedAddict</t>
+    <t>DQ2182</t>
+  </si>
+  <si>
+    <t>DQ2183</t>
+  </si>
+  <si>
+    <t>DQ2189</t>
+  </si>
+  <si>
+    <t>DQ2340</t>
+  </si>
+  <si>
+    <t>DPFCIN00</t>
+  </si>
+  <si>
+    <t>GPFCIN00</t>
+  </si>
+  <si>
+    <t>LikeMusic7</t>
+  </si>
+  <si>
+    <t>LikeTV7</t>
+  </si>
+  <si>
+    <t>LikeDrawing7</t>
+  </si>
+  <si>
+    <t>LikeComputer7</t>
+  </si>
+  <si>
+    <t>LikeOutSport7</t>
+  </si>
+  <si>
+    <t>LikeInSport7</t>
+  </si>
+  <si>
+    <t>FriendCount7</t>
+  </si>
+  <si>
+    <t>LikeFriendPlay7</t>
+  </si>
+  <si>
+    <t>LikeAlone7</t>
+  </si>
+  <si>
+    <t>FunFamily7</t>
+  </si>
+  <si>
+    <t>LikeSchool7</t>
+  </si>
+  <si>
+    <t>SadSchool7</t>
+  </si>
+  <si>
+    <t>TiredSchool7</t>
+  </si>
+  <si>
+    <t>FedSchool7</t>
+  </si>
+  <si>
+    <t>FriendTalk7</t>
+  </si>
+  <si>
+    <t>Bullied7</t>
+  </si>
+  <si>
+    <t>BullyOthers7</t>
+  </si>
+  <si>
+    <t>ChildLeftOut7</t>
+  </si>
+  <si>
+    <t>FightChildTeach7</t>
+  </si>
+  <si>
+    <t>Bullies others at school (age 7), asnwered by teacher</t>
+  </si>
+  <si>
+    <t>EverHomeless17</t>
+  </si>
+  <si>
+    <t>CurrHomeless17</t>
+  </si>
+  <si>
+    <t>MumCont17</t>
+  </si>
+  <si>
+    <t>MumSee17</t>
+  </si>
+  <si>
+    <t>MumSpeak17</t>
+  </si>
+  <si>
+    <t>DadSee17</t>
+  </si>
+  <si>
+    <t>DadCont17</t>
+  </si>
+  <si>
+    <t>DadSpeak17</t>
+  </si>
+  <si>
+    <t>agg_score17</t>
+  </si>
+  <si>
+    <t>AgeDepDiag17</t>
+  </si>
+  <si>
+    <t>DeprsTreatCurr17</t>
+  </si>
+  <si>
+    <t>DeprsTreat17</t>
+  </si>
+  <si>
+    <t>FirstCigAge17</t>
+  </si>
+  <si>
+    <t>FirstAlchAge17</t>
+  </si>
+  <si>
+    <t>FirstAlchDrinkAge17</t>
+  </si>
+  <si>
+    <t>AlchDrinkYr17</t>
+  </si>
+  <si>
+    <t>AlchDrinkMon17</t>
+  </si>
+  <si>
+    <t>AlchDrinkExcs17</t>
+  </si>
+  <si>
+    <t>AlchDrinkExcsNum17</t>
+  </si>
+  <si>
+    <t>AlchDrinkExcsAge17</t>
+  </si>
+  <si>
+    <t>EcstasyY/N17</t>
+  </si>
+  <si>
+    <t>SpeedY/N17</t>
+  </si>
+  <si>
+    <t>SemeronY/N17</t>
+  </si>
+  <si>
+    <t>KetamineY/N17</t>
+  </si>
+  <si>
+    <t>MephedroneY/N17</t>
+  </si>
+  <si>
+    <t>PsychoactiveY/N17</t>
+  </si>
+  <si>
+    <t>FriendSpend17</t>
+  </si>
+  <si>
+    <t>GamesSpend17</t>
+  </si>
+  <si>
+    <t>SocialmedSpend17</t>
+  </si>
+  <si>
+    <t>SocialmedAddict17</t>
+  </si>
+  <si>
+    <t>UpsetTeach7</t>
+  </si>
+  <si>
+    <t>Upset often at school, answred by teacher</t>
+  </si>
+  <si>
+    <t>Bullied at school, asnwered by teacher</t>
+  </si>
+  <si>
+    <t>ChildBullyTeach7</t>
+  </si>
+  <si>
+    <t>DepressionTeach7</t>
+  </si>
+  <si>
+    <t>Has drepression ,answeed by teacher</t>
+  </si>
+  <si>
+    <t>ParentsDiv7</t>
+  </si>
+  <si>
+    <t>Parents divorced at 7 years old</t>
+  </si>
+  <si>
+    <t>Parentsdiv17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parents divorced at 17 years old </t>
+  </si>
+  <si>
+    <t>MCSID</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>Child's Id</t>
+  </si>
+  <si>
+    <t>GCDRUA00</t>
+  </si>
+  <si>
+    <t>GCDRUB00</t>
+  </si>
+  <si>
+    <t>Have you ever taken any of the following? Cocaine</t>
+  </si>
+  <si>
+    <t>Have you ever taken any of the following? Cannabis</t>
+  </si>
+  <si>
+    <t>CannabisY/N17</t>
+  </si>
+  <si>
+    <t>CocaineY/N17</t>
+  </si>
+  <si>
+    <t>AcidY/N17</t>
   </si>
 </sst>
 </file>
@@ -525,12 +628,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -545,13 +654,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF800080"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8F8F8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </left>
+        <right style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </right>
+        <top style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </top>
+        <bottom style="thin">
+          <color theme="0" tint="-0.34998626667073579"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -827,10 +964,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J53"/>
+  <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -853,581 +990,697 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>175</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>176</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,B2:B53)</f>
-        <v>Age,Sex,LikeMusic,LikeTV,LikeDrawing,LikeComputer,LikeOutSport,LikeInSport,FriendCount,LikeFriendPlay,LikeAlone,FunFamily,LikeSchool,SadSchool,TiredSchool,FedSchool,FriendTalk,Bullied,BullyOthers,ChildLeftOut,EverHomeless,CurrHomeless,MumCont,MumSee,MumSpeak,DadCont,DadSee,DadSpeak,agg_score,AgeDepDiag,DeprsTreatCurr,DeprsTreat,FirstCigAge,FirstAlchAge,FirstAlchDrinkAge,AlchDrinkYr,AlchDrinkMon,AlchDrinkExcs,AlchDrinkExcsAge,AlchDrinkExcsNum,AcidY/N,EcstasyY/N,SpeedY/N,SemeronY/N,KetamineY/N,MephedroneY/N,PsychoactiveY/N,SpeedY/N,FriendSpend,GamesSpend,SocialmedSpend,SocialmedAddict</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="J3" t="e" cm="1">
+        <f t="array" aca="1" ref="J3" ca="1">A64(",",TRUE,B3:B56)</f>
+        <v>#REF!</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="C12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="C17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>131</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>133</v>
+        <v>141</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>134</v>
+        <v>140</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="C35" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="C36" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="C37" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C38" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="C39" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="C40" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>146</v>
+        <v>154</v>
       </c>
       <c r="C41" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
       <c r="C42" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>44</v>
+        <v>178</v>
       </c>
       <c r="B43" t="s">
-        <v>148</v>
+        <v>182</v>
       </c>
       <c r="C43" t="s">
-        <v>96</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>45</v>
+        <v>179</v>
       </c>
       <c r="B44" t="s">
-        <v>149</v>
+        <v>183</v>
       </c>
       <c r="C44" t="s">
-        <v>97</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>150</v>
+        <v>184</v>
       </c>
       <c r="C45" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
       <c r="C46" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="C47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C48" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="C49" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>154</v>
+        <v>159</v>
       </c>
       <c r="C50" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>155</v>
+        <v>160</v>
       </c>
       <c r="C51" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>156</v>
       </c>
       <c r="C52" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>161</v>
+      </c>
+      <c r="C53" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>162</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>163</v>
+      </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>54</v>
       </c>
-      <c r="B53" t="s">
-        <v>157</v>
-      </c>
-      <c r="C53" t="s">
+      <c r="B56" t="s">
+        <v>164</v>
+      </c>
+      <c r="C56" t="s">
         <v>106</v>
       </c>
     </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" t="s">
+        <v>133</v>
+      </c>
+      <c r="C57" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" t="s">
+        <v>165</v>
+      </c>
+      <c r="C58" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B59" t="s">
+        <v>168</v>
+      </c>
+      <c r="C59" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B60" t="s">
+        <v>169</v>
+      </c>
+      <c r="C60" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="C61" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B62" t="s">
+        <v>173</v>
+      </c>
+      <c r="C62" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,B2:B62)</f>
+        <v>Id,Age,Sex,LikeMusic7,LikeTV7,LikeDrawing7,LikeComputer7,LikeOutSport7,LikeInSport7,FriendCount7,LikeFriendPlay7,LikeAlone7,FunFamily7,LikeSchool7,SadSchool7,TiredSchool7,FedSchool7,FriendTalk7,Bullied7,BullyOthers7,ChildLeftOut7,EverHomeless17,CurrHomeless17,MumCont17,MumSee17,MumSpeak17,DadCont17,DadSee17,DadSpeak17,agg_score17,AgeDepDiag17,DeprsTreatCurr17,DeprsTreat17,FirstCigAge17,FirstAlchAge17,FirstAlchDrinkAge17,AlchDrinkYr17,AlchDrinkMon17,AlchDrinkExcs17,AlchDrinkExcsAge17,AlchDrinkExcsNum17,CannabisY/N17,CocaineY/N17,AcidY/N17,EcstasyY/N17,SpeedY/N17,SemeronY/N17,KetamineY/N17,MephedroneY/N17,PsychoactiveY/N17,SpeedY/N17,FriendSpend17,GamesSpend17,SocialmedSpend17,SocialmedAddict17,FightChildTeach7,UpsetTeach7,ChildBullyTeach7,DepressionTeach7,ParentsDiv7,Parentsdiv17</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,A2:A62)</f>
+        <v>MCSID,DCMCS4AGE,DCCSEX00,DCSC0001,DCSC0002,DCSC0003,DCSC0004,DCSC0005,DCSC0006,DCSC0007,DCSC0010,DCSC0015,DCSC0019,DCSC0021,DCSC0032,DCSC0033,DCSC0034,DCSC0035,DCSC0036,DCSC0037,DCSC0038,GCHOMS00,GCHOSS00,GCCOMO00,GCSEMA00,GCPHMA00,GCCOFA00,GCSEFA00,GCPHPA00,GCDEAN00,GCDAGE00,GCTRDE00,GCTRDV00,GCAGSM00,GCALCD00,GCALAG00,GCALCN00,GCALNF00,GCALFV00,GCAGFV00,GCALFN00,GCDRUA00,GCDRUB00,GCDRUC00,GCDRUD00,GCDRUL00,GCDRUS00,GCDRUI00,GCDRUJ00,GCDRUK00,GCSPFD00,GCTVHO00,GCCOMH00,GCSOME00,GCSOCM00,DQ2182,DQ2183,DQ2189,DQ2340,DPFCIN00,GPFCIN00</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A57:A61">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="MCSID">
+      <formula>NOT(ISERROR(SEARCH("MCSID",A57)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>